<commit_message>
change sx & sy in the table
</commit_message>
<xml_diff>
--- a/ipython_setup/startup/sample_example.xlsx
+++ b/ipython_setup/startup/sample_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pete\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1DE804-590C-4925-BBAD-774F625304EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C0AAC6-A386-4D41-961A-DCE2D532301A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32370" yWindow="2340" windowWidth="20610" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26115" yWindow="1905" windowWidth="20610" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample data" sheetId="1" r:id="rId1"/>
@@ -530,7 +530,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,10 +593,10 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>45.07</v>
+        <v>5.07</v>
       </c>
       <c r="C5">
-        <v>98.3</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -613,10 +613,10 @@
         <v>25</v>
       </c>
       <c r="B6">
-        <v>45.07</v>
+        <v>5.07</v>
       </c>
       <c r="C6">
-        <v>98.3</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -661,7 +661,7 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>0.1</v>

</xml_diff>